<commit_message>
Moved write and save function to parent class
</commit_message>
<xml_diff>
--- a/Templates.xlsx
+++ b/Templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousef\Desktop\Projects\MakePlus\Invoice Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAE82C7-8872-4F4B-A403-F45F2DE5A1FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82438475-DD16-4C01-967F-F4F3D9E7EEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MoreSpace" sheetId="1" r:id="rId1"/>
@@ -225,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -270,13 +270,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,6 +282,16 @@
     <xf numFmtId="7" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -612,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H47"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -662,7 +665,7 @@
       <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="32" t="s">
         <v>7</v>
       </c>
     </row>
@@ -694,7 +697,7 @@
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="28" t="s">
         <v>3</v>
       </c>
     </row>
@@ -702,7 +705,7 @@
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -714,8 +717,8 @@
       <c r="C22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="7" t="s">
         <v>15</v>
       </c>
@@ -724,11 +727,11 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="11"/>
       <c r="G23" s="12">
         <f>C23*F23</f>
@@ -737,11 +740,11 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="11"/>
       <c r="G24" s="12">
         <f>C24*F24</f>
@@ -750,11 +753,11 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="11"/>
       <c r="G25" s="12">
         <f t="shared" ref="G25:G33" si="0">C25*F25</f>
@@ -763,11 +766,11 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="11"/>
       <c r="G26" s="12">
         <f t="shared" si="0"/>
@@ -776,11 +779,11 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="11"/>
       <c r="G27" s="12">
         <f t="shared" si="0"/>
@@ -789,11 +792,11 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="11"/>
       <c r="G28" s="12">
         <f t="shared" si="0"/>
@@ -802,11 +805,11 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="11"/>
       <c r="G29" s="12">
         <f t="shared" si="0"/>
@@ -815,11 +818,11 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="11"/>
       <c r="G30" s="12">
         <f t="shared" si="0"/>
@@ -828,11 +831,11 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="11"/>
       <c r="G31" s="12">
         <f t="shared" si="0"/>
@@ -841,11 +844,11 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
       <c r="F32" s="11"/>
       <c r="G32" s="12">
         <f t="shared" si="0"/>
@@ -854,11 +857,11 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="11"/>
       <c r="G33" s="12">
         <f t="shared" si="0"/>
@@ -867,11 +870,11 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="11"/>
       <c r="G34" s="12">
         <f>C34*F34</f>
@@ -880,11 +883,11 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="11"/>
       <c r="G35" s="12">
         <f>C35*F35</f>
@@ -972,17 +975,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A29:B29"/>
@@ -999,6 +991,17 @@
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1009,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B1139E-6C38-4E54-A251-7E7CF79C803A}">
   <dimension ref="A2:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1063,7 +1066,7 @@
       <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="32" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1097,34 +1100,34 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="25"/>
+      <c r="B17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="25"/>
+      <c r="B21" s="22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
@@ -1134,8 +1137,8 @@
       <c r="C23" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="20" t="s">
         <v>15</v>
       </c>
@@ -1144,11 +1147,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="11"/>
       <c r="G24" s="12">
         <f>C24*F24</f>
@@ -1157,11 +1160,11 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="11"/>
       <c r="G25" s="12">
         <f>C25*F25</f>
@@ -1170,24 +1173,24 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="11"/>
       <c r="G26" s="12">
-        <f t="shared" ref="G26:G36" si="0">C26*F26</f>
+        <f t="shared" ref="G26:G35" si="0">C26*F26</f>
         <v>0</v>
       </c>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="11"/>
       <c r="G27" s="12">
         <f t="shared" si="0"/>
@@ -1196,11 +1199,11 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="11"/>
       <c r="G28" s="12">
         <f t="shared" si="0"/>
@@ -1209,11 +1212,11 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="11"/>
       <c r="G29" s="12">
         <f t="shared" si="0"/>
@@ -1222,11 +1225,11 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="11"/>
       <c r="G30" s="12">
         <f t="shared" si="0"/>
@@ -1235,25 +1238,25 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="11"/>
       <c r="G31" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H31" s="13"/>
-      <c r="J31" s="27"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
       <c r="F32" s="11"/>
       <c r="G32" s="12">
         <f t="shared" si="0"/>
@@ -1262,26 +1265,26 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="11"/>
       <c r="G33" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H33" s="13"/>
-      <c r="J33" s="28"/>
-      <c r="L33" s="29"/>
+      <c r="J33" s="25"/>
+      <c r="L33" s="26"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="11"/>
       <c r="G34" s="12">
         <f t="shared" si="0"/>
@@ -1290,11 +1293,11 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="11"/>
       <c r="G35" s="12">
         <f t="shared" si="0"/>
@@ -1303,17 +1306,17 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="11"/>
       <c r="G36" s="12">
         <f>C36*F36</f>
         <v>0</v>
       </c>
-      <c r="J36" s="30"/>
+      <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C37" s="9"/>
@@ -1323,9 +1326,9 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G38" s="14"/>
-      <c r="J38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="N38" s="29"/>
+      <c r="J38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="N38" s="26"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E39" s="5" t="s">
@@ -1371,8 +1374,8 @@
         <f>F42*G39</f>
         <v>0</v>
       </c>
-      <c r="J42" s="30"/>
-      <c r="L42" s="30"/>
+      <c r="J42" s="27"/>
+      <c r="L42" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E43" s="5" t="s">
@@ -1390,7 +1393,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L45" s="29"/>
+      <c r="L45" s="26"/>
     </row>
     <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
@@ -1398,12 +1401,31 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="23" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="A33:B33"/>
@@ -1412,25 +1434,6 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>